<commit_message>
Cherylyn's contribution to project
</commit_message>
<xml_diff>
--- a/data/Medals.xlsx
+++ b/data/Medals.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chery\Documents\mira-bing\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2DE53D9-D93D-4331-A173-B0D3BE3098E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Details" r:id="rId3" sheetId="1"/>
+    <sheet name="Details" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -461,11 +469,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -477,7 +484,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -495,18 +502,326 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -552,7 +867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -575,7 +890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -598,7 +913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -621,7 +936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -644,7 +959,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -667,7 +982,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -690,7 +1005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -713,7 +1028,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -736,7 +1051,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -759,7 +1074,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -782,7 +1097,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -805,7 +1120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -828,7 +1143,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -851,7 +1166,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -874,7 +1189,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -897,7 +1212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -920,7 +1235,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -943,7 +1258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -966,7 +1281,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -989,7 +1304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1012,7 +1327,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1035,7 +1350,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1058,7 +1373,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -1081,7 +1396,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1104,7 +1419,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1127,7 +1442,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -1150,7 +1465,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1173,7 +1488,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1196,7 +1511,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1219,7 +1534,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1242,7 +1557,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1265,7 +1580,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1288,7 +1603,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1311,7 +1626,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -1334,7 +1649,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -1357,7 +1672,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -1380,7 +1695,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -1403,7 +1718,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>74</v>
       </c>
@@ -1426,7 +1741,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -1449,7 +1764,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -1472,7 +1787,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -1495,7 +1810,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -1518,7 +1833,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -1541,7 +1856,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -1564,7 +1879,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -1587,7 +1902,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -1610,7 +1925,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -1633,7 +1948,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -1656,7 +1971,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -1679,7 +1994,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -1702,7 +2017,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -1725,7 +2040,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -1748,7 +2063,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -1771,7 +2086,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -1794,7 +2109,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -1817,7 +2132,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>111</v>
       </c>
@@ -1840,7 +2155,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -1863,7 +2178,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>111</v>
       </c>
@@ -1886,7 +2201,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -1909,7 +2224,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>117</v>
       </c>
@@ -1932,7 +2247,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>117</v>
       </c>
@@ -1955,7 +2270,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>117</v>
       </c>
@@ -1978,7 +2293,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>117</v>
       </c>
@@ -2001,7 +2316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>122</v>
       </c>
@@ -2024,7 +2339,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>122</v>
       </c>
@@ -2047,7 +2362,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>122</v>
       </c>
@@ -2070,7 +2385,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>126</v>
       </c>
@@ -2093,7 +2408,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>126</v>
       </c>
@@ -2116,7 +2431,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>126</v>
       </c>
@@ -2139,7 +2454,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>113</v>
       </c>
@@ -2162,7 +2477,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>113</v>
       </c>
@@ -2185,7 +2500,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>113</v>
       </c>
@@ -2208,7 +2523,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>113</v>
       </c>
@@ -2231,7 +2546,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>134</v>
       </c>
@@ -2254,7 +2569,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -2277,7 +2592,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>136</v>
       </c>
@@ -2300,7 +2615,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>136</v>
       </c>
@@ -2323,7 +2638,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>140</v>
       </c>
@@ -2346,7 +2661,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>140</v>
       </c>
@@ -2369,7 +2684,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>140</v>
       </c>
@@ -2392,7 +2707,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>140</v>
       </c>
@@ -2415,7 +2730,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>140</v>
       </c>
@@ -2438,7 +2753,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>140</v>
       </c>
@@ -2461,7 +2776,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>140</v>
       </c>
@@ -2485,6 +2800,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>